<commit_message>
menambah modul butir sikap kur13
</commit_message>
<xml_diff>
--- a/public/template/template_guru.xlsx
+++ b/public/template/template_guru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WEB PROJEK\LARAVEL 11\madrasah-app-v2\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B10AB8C-5641-473C-BDE7-923A339E058A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC64E94-D389-4D38-B97B-A3D7051E2234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,12 +361,13 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="22.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -446,6 +447,14 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Nama Lengkap" prompt="Nama lengkap wajib disi" sqref="B2:B60" xr:uid="{537828D3-6FB8-4ED0-9D8D-E02C89D163E0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Gelar Belakang" prompt="Masukan gelar belakang contoh S.Pd.I" sqref="D2:D63" xr:uid="{714B5709-4BE5-41B7-924D-68437758AC8F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="NIK" prompt="Masukkan 16 digit angka " sqref="E2:E267" xr:uid="{9EB306FF-5D0E-400B-9838-8D16988A5925}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Jenis Kelamin" prompt="Laki-laki atau Perempuan" sqref="F2:F37" xr:uid="{FD42FE39-7CB0-46E5-8D76-40D53D78DE30}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tanggal Lahir" prompt="Masukan dalam format text dengan contoh 2000-07-01" sqref="H2:H115" xr:uid="{CEC9BFC8-74F0-40AD-8783-91DF611EAB18}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Tanggal" prompt="Masukkan format YYY-MM-DD atau 2000-07-01" sqref="L2:M46" xr:uid="{5567B315-1258-4724-A1BD-8A4B28768AA4}"/>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>

</xml_diff>